<commit_message>
Added Apple Watch and Modified Arduino Code
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">Variables--&gt;</t>
   </si>
@@ -31,16 +31,7 @@
     <t xml:space="preserve">Experiment</t>
   </si>
   <si>
-    <t xml:space="preserve">Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hit Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequency of Telemetry Data Transmission (continuous only) - Timeout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch No.</t>
+    <t xml:space="preserve">Device ID</t>
   </si>
   <si>
     <t xml:space="preserve">NetworkProfile</t>
@@ -49,6 +40,12 @@
     <t xml:space="preserve">Duration</t>
   </si>
   <si>
+    <t xml:space="preserve">Payload Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period</t>
+  </si>
+  <si>
     <t xml:space="preserve">Profile</t>
   </si>
   <si>
@@ -73,7 +70,7 @@
     <t xml:space="preserve">EP001</t>
   </si>
   <si>
-    <t xml:space="preserve">onDemand</t>
+    <t xml:space="preserve">Shams_run2</t>
   </si>
   <si>
     <t xml:space="preserve">2G-DevelopingRural</t>
@@ -215,7 +212,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,31 +309,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF107"/>
+  <dimension ref="A1:AC107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="14" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -346,84 +341,80 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="Z1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="Y1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="AA1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="str">
-        <f aca="false">IF(D2="OnDemand","ExperimentA","ExperimentB")</f>
-        <v>ExperimentA</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="1" t="n">
+        <v>130000</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="4" t="n">
         <v>10000</v>
       </c>
-      <c r="G2" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>130000</v>
-      </c>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="Z2" s="5" t="s">
-        <v>18</v>
+      <c r="W2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="6" t="n">
+        <v>650</v>
+      </c>
+      <c r="Y2" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="6" t="n">
+        <v>20</v>
       </c>
       <c r="AA2" s="6" t="n">
         <v>650</v>
@@ -432,15 +423,6 @@
         <v>2</v>
       </c>
       <c r="AC2" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD2" s="6" t="n">
-        <v>650</v>
-      </c>
-      <c r="AE2" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="6" t="n">
         <v>18</v>
       </c>
     </row>
@@ -448,100 +430,94 @@
       <c r="B3" s="1"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
-      <c r="AA26" s="7"/>
-      <c r="AB26" s="8"/>
+      <c r="Y26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="8"/>
+      <c r="Y27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="7"/>
-      <c r="AB28" s="8"/>
+      <c r="Y28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="8"/>
+      <c r="Y29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="8"/>
+      <c r="Y30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="8"/>
+      <c r="Y31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="8"/>
+      <c r="Y32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="8"/>
+      <c r="Y33" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E14" type="list">
       <formula1>"3G-Good,3G-Average,Edge-Lossy,Edge-Average,Edge-Good,2G-DevelopingRural,2G-DevelopingUrban"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Version 4 Audio test added
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -70,16 +70,16 @@
     <t xml:space="preserve">Upload - Bandwidth Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">EP003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ayesh_Test2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phy-wifi-baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baseline</t>
+    <t xml:space="preserve">EP001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayesh_test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2G-DevelopingUrban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">2G-DevelopingRural</t>
@@ -321,15 +321,15 @@
   <dimension ref="A1:AC105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.78"/>
@@ -400,7 +400,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -410,7 +410,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="n">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
@@ -438,6 +438,116 @@
       <c r="AC2" s="6" t="n">
         <v>18</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T24" s="7"/>
@@ -505,12 +615,8 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E12" type="list">
-      <formula1>"3G-Good,3G-Average,Edge-Lossy,Edge-Average,Edge-Good,2G-DevelopingRural,2G-DevelopingUrban"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2" type="list">
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E13" type="list">
       <formula1>"3G-Good,3G-Average,Edge-Lossy,Edge-Average,Edge-Good,2G-DevelopingRural,2G-DevelopingUrban,Phy-wifi-baseline"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Updated test Automator process
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Variables--&gt;</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">watch</t>
   </si>
   <si>
+    <t xml:space="preserve">periodic/poisson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Profile</t>
   </si>
   <si>
@@ -91,13 +94,16 @@
     <t xml:space="preserve">Phy-wifi-baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">normal</t>
+    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">hrm</t>
   </si>
   <si>
-    <t xml:space="preserve">galaxy watch</t>
+    <t xml:space="preserve">Samsung-Gear-s3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poisson</t>
   </si>
   <si>
     <t xml:space="preserve">2G-DevelopingRural</t>
@@ -110,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +156,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -222,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,6 +251,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,7 +263,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,8 +358,8 @@
   </sheetPr>
   <dimension ref="A1:AB105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -350,11 +370,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="13" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="16" style="0" width="10.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -392,270 +415,289 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4"/>
       <c r="V1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1800000</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="4" t="n">
-        <v>500</v>
+      <c r="H2" s="5" t="n">
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="6" t="n">
+      <c r="N2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="8" t="n">
         <v>650</v>
       </c>
-      <c r="X2" s="6" t="n">
+      <c r="X2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="Y2" s="6" t="n">
+      <c r="Y2" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="Z2" s="6" t="n">
+      <c r="Z2" s="8" t="n">
         <v>650</v>
       </c>
-      <c r="AA2" s="6" t="n">
+      <c r="AA2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AB2" s="6" t="n">
+      <c r="AB2" s="8" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="8"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="8"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="8"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="8"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="8"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="8"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="8"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="8"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="10"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E13" type="list">
       <formula1>"3G-Good,3G-Average,Edge-Lossy,Edge-Average,Edge-Good,2G-DevelopingRural,2G-DevelopingUrban,Phy-wifi-baseline"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="list">
+      <formula1>"periodic,poisson"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
+      <formula1>"sensor_local,sensor_offload,audio,c_audio,offload,text,text_offload"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+      <formula1>"Samsung-Gear-s3,Galaxy-Watch,Huawei-Watch 2,Fitbit-Versa,Apple-Watch"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
December Progress + Text Model
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Phy-wifi-baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
+    <t xml:space="preserve">text_offload</t>
   </si>
   <si>
     <t xml:space="preserve">hrm</t>
@@ -359,7 +359,7 @@
   <dimension ref="A1:AB105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,7 +447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
@@ -461,11 +461,11 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>1800000</v>
+        <v>3600000</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="5" t="n">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>24</v>
@@ -474,7 +474,7 @@
         <v>25</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>2</v>
@@ -692,12 +692,12 @@
       <formula1>"periodic,poisson"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
-      <formula1>"sensor_local,sensor_offload,audio,c_audio,offload,text,text_offload"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+      <formula1>"Samsung-Gear-s3,Galaxy-Watch,Huawei-Watch 2,Fitbit-Versa,Apple-Watch"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
-      <formula1>"Samsung-Gear-s3,Galaxy-Watch,Huawei-Watch 2,Fitbit-Versa,Apple-Watch"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
+      <formula1>"sensor_local,sensor_offload,audio,c_audio,offload,text_local,text_offload"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>